<commit_message>
SAP code in resources
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CD69C7-B067-4839-899F-FAC3B53E4947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2947020-77C8-4A1E-BF45-E92817DE603F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Precios!$A$2:$M$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AH$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AI$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
   <si>
     <t>Code</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Booking_fee</t>
+  </si>
+  <si>
+    <t>Código SAP</t>
+  </si>
+  <si>
+    <t>SAP_code</t>
   </si>
 </sst>
 </file>
@@ -875,7 +881,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -883,31 +889,31 @@
   <cols>
     <col min="1" max="2" width="37.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="9.5703125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="15.42578125" style="2" customWidth="1"/>
-    <col min="26" max="26" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" style="2" customWidth="1"/>
-    <col min="29" max="29" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="16.85546875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="20.5703125" style="2" customWidth="1"/>
-    <col min="35" max="35" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="24.85546875" style="2"/>
+    <col min="4" max="5" width="20.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="9.5703125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.42578125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" style="2" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="16.85546875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="20.5703125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -918,100 +924,103 @@
         <v>33</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AJ1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1022,84 +1031,87 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1109,42 +1121,42 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="16"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AI$1&amp;LEFT($C3,6)&amp;$F3&amp;$H3,Precios!$R:$R,Precios!H:H,0)*_xlfn.XLOOKUP($M3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($J3,".",",")))</f>
+      <c r="N3" s="10"/>
+      <c r="O3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AJ$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!H:H,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="O3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AI$1&amp;LEFT($C3,6)&amp;$F3&amp;$H3,Precios!$R:$R,Precios!I:I,0)*_xlfn.XLOOKUP($M3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($J3,".",",")))</f>
+      <c r="P3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AJ$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!I:I,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="P3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AI$1&amp;LEFT($C3,6)&amp;$F3&amp;$H3,Precios!$R:$R,Precios!J:J,0)*_xlfn.XLOOKUP($M3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($J3,".",",")))</f>
+      <c r="Q3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AJ$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!J:J,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AI$1&amp;LEFT($C3,6)&amp;$F3&amp;$H3,Precios!$R:$R,Precios!K:K,0)</f>
+      <c r="R3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AJ$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!K:K,0)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="13">
-        <f t="shared" ref="R3" ca="1" si="0">$N3+$Q3</f>
+      <c r="S3" s="13">
+        <f t="shared" ref="S3" ca="1" si="0">$O3+$R3</f>
         <v>0</v>
       </c>
-      <c r="S3" s="13">
-        <f t="shared" ref="S3" ca="1" si="1">$O3+$Q3</f>
+      <c r="T3" s="13">
+        <f t="shared" ref="T3" ca="1" si="1">$P3+$R3</f>
         <v>0</v>
       </c>
-      <c r="T3" s="13">
-        <f t="shared" ref="T3" ca="1" si="2">$P3+$Q3</f>
+      <c r="U3" s="13">
+        <f t="shared" ref="U3" ca="1" si="2">$Q3+$R3</f>
         <v>0</v>
       </c>
-      <c r="U3" s="14"/>
-      <c r="V3" s="15"/>
+      <c r="V3" s="14"/>
       <c r="W3" s="15"/>
-      <c r="X3" s="10"/>
+      <c r="X3" s="15"/>
       <c r="Y3" s="10"/>
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
@@ -1155,10 +1167,11 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AH3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AH9999">
+  <autoFilter ref="A2:AI3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AI9999">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>LEN($C3)=12</formula>
     </cfRule>
@@ -1360,6 +1373,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
@@ -1368,15 +1390,6 @@
     <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1577,20 +1590,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
     <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Resource additional LAU data
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB41D266-6E77-40C4-B700-5D298C0EEAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAE1329-D9B4-4233-9009-782BF971D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,9 +19,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Precios!$A$2:$M$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AJ$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AR$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Code</t>
   </si>
@@ -316,6 +316,56 @@
   </si>
   <si>
     <t>Management fee</t>
+  </si>
+  <si>
+    <t>Ref. Catastro</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Registry_code</t>
+  </si>
+  <si>
+    <t>Resource_usage.Name</t>
+  </si>
+  <si>
+    <t>Post
+CAPEX</t>
+  </si>
+  <si>
+    <t>Pre
+CAPEX</t>
+  </si>
+  <si>
+    <t>Pre_capex</t>
+  </si>
+  <si>
+    <t>Post_capex</t>
+  </si>
+  <si>
+    <t>Contrato luz</t>
+  </si>
+  <si>
+    <t>Contrato agua</t>
+  </si>
+  <si>
+    <t>Contrato gas</t>
+  </si>
+  <si>
+    <t>Contract_electricity</t>
+  </si>
+  <si>
+    <t>Contract_water</t>
+  </si>
+  <si>
+    <t>Contract_gas</t>
+  </si>
+  <si>
+    <t>Interior</t>
+  </si>
+  <si>
+    <t>Int/Ext</t>
   </si>
 </sst>
 </file>
@@ -453,7 +503,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,6 +539,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -887,7 +939,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -909,18 +961,22 @@
     <col min="16" max="22" width="9.5703125" style="2" customWidth="1"/>
     <col min="23" max="23" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="15.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" style="2" customWidth="1"/>
-    <col min="31" max="31" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="16.85546875" style="2" customWidth="1"/>
-    <col min="36" max="36" width="20.5703125" style="2" customWidth="1"/>
-    <col min="37" max="37" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="24.85546875" style="2"/>
+    <col min="26" max="26" width="39.140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="24.7109375" style="2" customWidth="1"/>
+    <col min="28" max="29" width="11.85546875" style="2" customWidth="1"/>
+    <col min="30" max="32" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15.42578125" style="2" customWidth="1"/>
+    <col min="35" max="35" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="2" customWidth="1"/>
+    <col min="38" max="39" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="43" width="16.85546875" style="2" customWidth="1"/>
+    <col min="44" max="44" width="20.5703125" style="2" customWidth="1"/>
+    <col min="45" max="45" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -993,44 +1049,68 @@
         <v>76</v>
       </c>
       <c r="Z1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AS1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2024</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1091,40 +1171,64 @@
         <v>80</v>
       </c>
       <c r="Z2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1141,19 +1245,19 @@
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AK$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!H:H,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!H:H,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AK$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!I:I,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!I:I,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="R3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AK$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!J:J,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!J:J,0)*_xlfn.XLOOKUP($N3,Tarifas!$A:$A,Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AK$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!K:K,0)</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,Precios!$R:$R,Precios!K:K,0)</f>
         <v>0</v>
       </c>
       <c r="T3" s="13">
@@ -1171,21 +1275,29 @@
       <c r="W3" s="14"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AJ3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AJ9999">
+  <autoFilter ref="A2:AR3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AR9999">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>LEN($C3)=12</formula>
     </cfRule>
@@ -1387,6 +1499,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -1583,27 +1715,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1620,23 +1751,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Specify resource type on load report
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09320602-C6FA-4135-A839-69AC93CFAEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC5EEA-99FF-49A3-88C9-100F29EFA8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="37" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">_Precios!$A$2:$M$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estados!$A$2:$A$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AO$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AP$3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t>Code</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>Status.Name</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Resource_type</t>
   </si>
 </sst>
 </file>
@@ -942,42 +948,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="37.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="22" width="9.5703125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="39.140625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" style="2" customWidth="1"/>
-    <col min="25" max="26" width="11.85546875" style="2" customWidth="1"/>
-    <col min="27" max="29" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="15.42578125" style="2" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" style="2" customWidth="1"/>
-    <col min="35" max="36" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="16.85546875" style="2" customWidth="1"/>
-    <col min="41" max="41" width="20.5703125" style="2" customWidth="1"/>
-    <col min="42" max="42" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="24.85546875" style="2"/>
+    <col min="3" max="4" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="23" width="9.5703125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="39.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="24.7109375" style="2" customWidth="1"/>
+    <col min="26" max="27" width="11.85546875" style="2" customWidth="1"/>
+    <col min="28" max="30" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.42578125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.7109375" style="2" customWidth="1"/>
+    <col min="36" max="37" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="16.85546875" style="2" customWidth="1"/>
+    <col min="42" max="42" width="20.5703125" style="2" customWidth="1"/>
+    <col min="43" max="43" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -985,124 +991,127 @@
         <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AQ1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1110,108 +1119,111 @@
         <v>69</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="4"/>
+      <c r="X2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1222,47 +1234,47 @@
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="14"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AP$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($N3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AQ$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AP$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($N3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+      <c r="R3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AQ$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="R3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AP$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($N3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($K3,".",",")))</f>
+      <c r="S3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AQ$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
-      <c r="S3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AP$1&amp;LEFT($C3,6)&amp;$G3&amp;$I3,_Precios!$R:$R,_Precios!K:K,0)</f>
+      <c r="T3" s="13">
+        <f ca="1">_xlfn.XLOOKUP($AQ$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!K:K,0)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="13">
-        <f t="shared" ref="T3" ca="1" si="0">$P3+$S3</f>
+      <c r="U3" s="13">
+        <f t="shared" ref="U3" ca="1" si="0">$Q3+$T3</f>
         <v>0</v>
       </c>
-      <c r="U3" s="13">
-        <f t="shared" ref="U3" ca="1" si="1">$Q3+$S3</f>
+      <c r="V3" s="13">
+        <f t="shared" ref="V3" ca="1" si="1">$R3+$T3</f>
         <v>0</v>
       </c>
-      <c r="V3" s="13">
-        <f t="shared" ref="V3" ca="1" si="2">$R3+$S3</f>
+      <c r="W3" s="13">
+        <f t="shared" ref="W3" ca="1" si="2">$S3+$T3</f>
         <v>0</v>
       </c>
-      <c r="W3" s="17"/>
       <c r="X3" s="17"/>
-      <c r="Y3" s="18"/>
+      <c r="Y3" s="17"/>
       <c r="Z3" s="18"/>
       <c r="AA3" s="18"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="18"/>
-      <c r="AD3" s="10"/>
+      <c r="AD3" s="18"/>
       <c r="AE3" s="10"/>
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
@@ -1274,12 +1286,13 @@
       <c r="AM3" s="10"/>
       <c r="AN3" s="10"/>
       <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AO3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AO9999">
+  <autoFilter ref="A2:AP3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AP9999">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>LEN($C3)=12</formula>
+      <formula>LEN($D3)=12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1292,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D6A7EA-EF6A-4647-BD82-04BF3857C227}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1539,6 +1552,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -1735,27 +1768,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1772,23 +1804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Resources registry # and date
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38861D8-3348-43D3-AB05-90D8069FB832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34066A5-F297-4520-B5C9-8670D9E63C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">_Precios!$A$2:$M$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estados!$A$2:$A$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AS$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AT$3</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
   <si>
     <t>Code</t>
   </si>
@@ -308,15 +308,9 @@
     <t>Management fee</t>
   </si>
   <si>
-    <t>Ref. Catastro</t>
-  </si>
-  <si>
     <t>Uso</t>
   </si>
   <si>
-    <t>Registry_code</t>
-  </si>
-  <si>
     <t>Resource_usage.Name</t>
   </si>
   <si>
@@ -396,6 +390,18 @@
   </si>
   <si>
     <t>Post-CAPEX</t>
+  </si>
+  <si>
+    <t>Nº de registro</t>
+  </si>
+  <si>
+    <t>Fecha de registro</t>
+  </si>
+  <si>
+    <t>Registry_num</t>
+  </si>
+  <si>
+    <t>Registry_date</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,6 +579,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -972,7 +980,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT3"/>
+  <dimension ref="A1:AU4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -992,24 +1000,25 @@
     <col min="15" max="15" width="20.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="23" width="9.5703125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="39.140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="24.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" style="2" customWidth="1"/>
-    <col min="27" max="29" width="12.140625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="11.85546875" style="2" customWidth="1"/>
-    <col min="31" max="33" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="15.42578125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.7109375" style="2" customWidth="1"/>
-    <col min="39" max="40" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="44" width="16.85546875" style="2" customWidth="1"/>
-    <col min="45" max="45" width="20.5703125" style="2" customWidth="1"/>
-    <col min="46" max="46" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="24.85546875" style="2"/>
+    <col min="24" max="24" width="30" style="2" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="24.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" style="2" customWidth="1"/>
+    <col min="28" max="30" width="12.140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" style="2" customWidth="1"/>
+    <col min="32" max="34" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="15.42578125" style="2" customWidth="1"/>
+    <col min="37" max="37" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" style="2" customWidth="1"/>
+    <col min="40" max="41" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="45" width="16.85546875" style="2" customWidth="1"/>
+    <col min="46" max="46" width="20.5703125" style="2" customWidth="1"/>
+    <col min="47" max="47" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1017,7 +1026,7 @@
         <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>33</v>
@@ -1076,77 +1085,80 @@
         <v>73</v>
       </c>
       <c r="X1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AF1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="AO1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AT1" s="1">
+      <c r="AU1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -1201,73 +1213,76 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="Y2" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AA2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AG2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1285,19 +1300,19 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AU$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="R3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AU$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AU$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="T3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!K:K,0)</f>
+        <f ca="1">_xlfn.XLOOKUP($AU$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!K:K,0)</f>
         <v>0</v>
       </c>
       <c r="U3" s="13">
@@ -1312,14 +1327,16 @@
         <f t="shared" ref="W3" ca="1" si="2">$S3+$T3</f>
         <v>0</v>
       </c>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="18"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z3" s="17"/>
       <c r="AA3" s="18"/>
       <c r="AB3" s="18"/>
       <c r="AC3" s="18"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="10"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="20"/>
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
@@ -1334,10 +1351,14 @@
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
       <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="Y4" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AS3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AS9999">
+  <autoFilter ref="A2:AT3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AT9999">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>LEN($D3)=12</formula>
     </cfRule>
@@ -1373,30 +1394,30 @@
         <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -1599,6 +1620,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -1795,27 +1836,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1832,23 +1872,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Report resources valuation change
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD63C75-C8CB-4220-AA68-FFA865304360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFDF5B9-B8E5-495C-9701-118E781FE26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="37" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">_Precios!$A$2:$M$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estados!$A$2:$A$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AV$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AR$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Valoraciones!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="125">
   <si>
     <t>Code</t>
   </si>
@@ -1009,9 +1009,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1033,22 +1033,20 @@
     <col min="25" max="25" width="10.7109375" style="2" customWidth="1"/>
     <col min="26" max="26" width="30" style="2" customWidth="1"/>
     <col min="27" max="27" width="24.7109375" style="2" customWidth="1"/>
-    <col min="28" max="28" width="11.85546875" style="2" customWidth="1"/>
-    <col min="29" max="32" width="14.7109375" style="2" customWidth="1"/>
-    <col min="33" max="33" width="11.85546875" style="2" customWidth="1"/>
-    <col min="34" max="36" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="15.42578125" style="2" customWidth="1"/>
-    <col min="39" max="39" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.7109375" style="2" customWidth="1"/>
-    <col min="42" max="43" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="47" width="16.85546875" style="2" customWidth="1"/>
-    <col min="48" max="48" width="20.5703125" style="2" customWidth="1"/>
-    <col min="49" max="49" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="24.85546875" style="2"/>
+    <col min="28" max="29" width="11.85546875" style="2" customWidth="1"/>
+    <col min="30" max="32" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15.42578125" style="2" customWidth="1"/>
+    <col min="35" max="35" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="2" customWidth="1"/>
+    <col min="38" max="39" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="43" width="16.85546875" style="2" customWidth="1"/>
+    <col min="44" max="44" width="20.5703125" style="2" customWidth="1"/>
+    <col min="45" max="45" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1130,71 +1128,59 @@
         <v>106</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="AH1" s="3" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="AN1" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="AP1" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AV1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="1">
+      <c r="AS1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1264,67 +1250,55 @@
         <v>107</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AO2" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1342,19 +1316,19 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AW$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="R3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AW$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AW$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="T3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AW$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!K:K,0)</f>
+        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$R:$R,_Precios!K:K,0)</f>
         <v>0</v>
       </c>
       <c r="U3" s="13">
@@ -1376,11 +1350,11 @@
       <c r="Z3" s="21"/>
       <c r="AA3" s="17"/>
       <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10"/>
@@ -1392,14 +1366,10 @@
       <c r="AP3" s="10"/>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-      <c r="AV3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AV3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AV9991">
+  <autoFilter ref="A2:AR3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AR9991">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>LEN($D3)=12</formula>
     </cfRule>
@@ -1474,7 +1444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1D64B2-929E-46C9-92E4-4B6A6392A32E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1738,6 +1708,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -1934,17 +1915,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1955,6 +1925,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1973,17 +1954,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Group base prices resources report
</commit_message>
<xml_diff>
--- a/app/templates/report/recursos.xlsx
+++ b/app/templates/report/recursos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56CBDCF-46D6-4E65-B960-D63A6EEC13D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665ED486-A6EB-4E3F-9C4D-FABA78B3DD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="37" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">_Precios!$A$2:$N$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Estados!$A$2:$A$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AR$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Recursos!$A$2:$AS$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Valoraciones!$A$2:$A$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
   <si>
     <t>Code</t>
   </si>
@@ -1015,9 +1015,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1034,25 +1034,25 @@
     <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="23" width="9.5703125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="30" style="2" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="30" style="2" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" style="2" customWidth="1"/>
-    <col min="28" max="29" width="11.85546875" style="2" customWidth="1"/>
-    <col min="30" max="32" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="15.42578125" style="2" customWidth="1"/>
-    <col min="35" max="35" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" style="2" customWidth="1"/>
-    <col min="38" max="39" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="16.85546875" style="2" customWidth="1"/>
-    <col min="44" max="44" width="20.5703125" style="2" customWidth="1"/>
-    <col min="45" max="45" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="24.85546875" style="2"/>
+    <col min="17" max="24" width="9.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="30" style="2" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="30" style="2" customWidth="1"/>
+    <col min="28" max="28" width="24.7109375" style="2" customWidth="1"/>
+    <col min="29" max="30" width="11.85546875" style="2" customWidth="1"/>
+    <col min="31" max="33" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="15.42578125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" style="2" customWidth="1"/>
+    <col min="39" max="40" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="16.85546875" style="2" customWidth="1"/>
+    <col min="45" max="45" width="20.5703125" style="2" customWidth="1"/>
+    <col min="46" max="46" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1107,86 +1107,89 @@
         <v>64</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AT1" s="1">
         <f ca="1">IF(MONTH(TODAY())&gt;8,1+YEAR(TODAY()),YEAR(TODAY()))</f>
         <v>2025</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1240,71 +1243,72 @@
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -1322,42 +1326,45 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!H:H,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="R3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!I:I,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="S3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
+        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!J:J,0)*_xlfn.XLOOKUP($O3,_Tarifas!$A:$A,_Tarifas!C:C,0)*(1+0.01*_xlfn.NUMBERVALUE(SUBSTITUTE($L3,".",",")))</f>
         <v>0</v>
       </c>
       <c r="T3" s="13">
-        <f ca="1">_xlfn.XLOOKUP($AS$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!L:L,0)</f>
+        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!K:K,0)</f>
         <v>0</v>
       </c>
       <c r="U3" s="13">
-        <f t="shared" ref="U3" ca="1" si="0">$Q3+$T3</f>
+        <f ca="1">_xlfn.XLOOKUP($AT$1&amp;LEFT($D3,6)&amp;$H3&amp;$J3,_Precios!$S:$S,_Precios!L:L,0)</f>
         <v>0</v>
       </c>
       <c r="V3" s="13">
-        <f t="shared" ref="V3" ca="1" si="1">$R3+$T3</f>
+        <f t="shared" ref="V3" ca="1" si="0">$Q3+$U3</f>
         <v>0</v>
       </c>
       <c r="W3" s="13">
-        <f t="shared" ref="W3" ca="1" si="2">$S3+$T3</f>
+        <f t="shared" ref="W3" ca="1" si="1">$R3+$U3</f>
         <v>0</v>
       </c>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="19" t="s">
+      <c r="X3" s="13">
+        <f t="shared" ref="X3" ca="1" si="2">$S3+$U3</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="10"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="20"/>
       <c r="AE3" s="10"/>
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
@@ -1372,10 +1379,11 @@
       <c r="AP3" s="10"/>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AR3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A3:AR9991">
+  <autoFilter ref="A2:AS3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A3:AS9991">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>LEN($D3)=12</formula>
     </cfRule>
@@ -1527,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F063E8C-9C12-4A86-8416-6A77642A363A}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1721,6 +1729,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -1917,17 +1936,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1938,6 +1946,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1956,17 +1975,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
   <ds:schemaRefs>

</xml_diff>